<commit_message>
pag 190 ejer 7
</commit_message>
<xml_diff>
--- a/pag190ejer4.xlsx
+++ b/pag190ejer4.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2DAW\Empressa Iniciativa DAW Diurno\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8924A7-35AE-4D15-8B03-D06EEC2AD647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja3" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
   <si>
     <t>activo</t>
   </si>
@@ -72,13 +78,31 @@
   </si>
   <si>
     <t>REALIZABLE</t>
+  </si>
+  <si>
+    <t>Fondo de maniobra</t>
+  </si>
+  <si>
+    <t>pasivo corriente</t>
+  </si>
+  <si>
+    <t>ratio de  liquidez</t>
+  </si>
+  <si>
+    <t>activo corriente</t>
+  </si>
+  <si>
+    <t>ratio de  endeudamiento</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,6 +118,13 @@
     </font>
     <font>
       <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -151,44 +182,45 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -478,437 +510,280 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="1.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="13" width="14.140625" style="6" hidden="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="25.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="5" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" customWidth="1"/>
+    <col min="5" max="12" width="14.140625" hidden="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" customWidth="1"/>
+    <col min="14" max="14" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="19.5" customHeight="1">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="9" t="s">
+    <row r="1" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="O1" s="10"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="9" t="s">
+      <c r="O1" s="4"/>
+      <c r="Q1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="10"/>
-    </row>
-    <row r="2" spans="1:18" ht="19.5" customHeight="1">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1" t="s">
+      <c r="R1" s="4"/>
+    </row>
+    <row r="2" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N2" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="4">
+      <c r="O2" s="6">
         <v>1000</v>
       </c>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="4">
+      <c r="R2" s="6">
         <v>5000</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="19.5" customHeight="1">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1" t="s">
+    <row r="3" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N3" t="s">
         <v>4</v>
       </c>
-      <c r="O3" s="4">
+      <c r="O3" s="6">
         <v>2500</v>
       </c>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" t="s">
         <v>5</v>
       </c>
-      <c r="R3" s="3">
+      <c r="R3" s="8">
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="19.5" customHeight="1">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1" t="s">
+    <row r="4" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N4" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="4">
+      <c r="O4" s="6">
         <v>3000</v>
       </c>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1" t="s">
+      <c r="Q4" t="s">
         <v>7</v>
       </c>
-      <c r="R4" s="4">
+      <c r="R4" s="6">
         <v>5000</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="19.5" customHeight="1">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1" t="s">
+    <row r="5" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N5" t="s">
         <v>8</v>
       </c>
-      <c r="O5" s="4">
+      <c r="O5" s="6">
         <v>1500</v>
       </c>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1" t="s">
+      <c r="Q5" t="s">
         <v>9</v>
       </c>
-      <c r="R5" s="4"/>
-    </row>
-    <row r="6" spans="1:18" ht="19.5" customHeight="1">
-      <c r="A6" s="1" t="s">
+      <c r="R5" s="6"/>
+    </row>
+    <row r="6" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="6">
         <v>1000</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1" t="s">
+      <c r="N6" t="s">
         <v>10</v>
       </c>
-      <c r="O6" s="4">
+      <c r="O6" s="6">
         <v>4000</v>
       </c>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1" t="s">
+      <c r="Q6" t="s">
         <v>11</v>
       </c>
-      <c r="R6" s="4">
+      <c r="R6" s="6">
         <v>5000</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="19.5" customHeight="1">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="6">
         <v>5000</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1" t="s">
+      <c r="N7" t="s">
         <v>12</v>
       </c>
-      <c r="O7" s="4">
+      <c r="O7" s="6">
         <v>5000</v>
       </c>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1" t="s">
+      <c r="Q7" t="s">
         <v>13</v>
       </c>
-      <c r="R7" s="4">
+      <c r="R7" s="6">
         <f>SUM(R2:R6)</f>
         <v>17000</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="19.5" customHeight="1">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="6">
         <v>2500</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1" t="s">
+      <c r="N8" t="s">
         <v>14</v>
       </c>
-      <c r="O8" s="4">
+      <c r="O8" s="6">
         <f>SUM(O2:O7)</f>
         <v>17000</v>
       </c>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="5"/>
-    </row>
-    <row r="9" spans="1:18" ht="19.5" customHeight="1">
-      <c r="A9" s="1" t="s">
+    </row>
+    <row r="9" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="6">
         <v>3000</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="5"/>
-    </row>
-    <row r="10" spans="1:18" ht="19.5" customHeight="1">
-      <c r="A10" s="1" t="s">
+    </row>
+    <row r="10" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="6">
         <v>1500</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="5"/>
-    </row>
-    <row r="11" spans="1:18" ht="19.5" customHeight="1">
-      <c r="A11" s="1" t="s">
+    </row>
+    <row r="11" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="6">
         <v>4000</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="5"/>
-    </row>
-    <row r="12" spans="1:18" ht="19.5" customHeight="1">
-      <c r="A12" s="1" t="s">
+    </row>
+    <row r="12" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="6">
         <v>5000</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="5"/>
-    </row>
-    <row r="13" spans="1:18" ht="19.5" customHeight="1">
-      <c r="A13" s="1" t="s">
+    </row>
+    <row r="13" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="6">
         <v>2000</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="5"/>
-    </row>
-    <row r="14" spans="1:18" ht="19.5" customHeight="1">
-      <c r="A14" s="1" t="s">
+    </row>
+    <row r="14" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="6">
         <v>5000</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="5"/>
-    </row>
-    <row r="15" spans="1:18" ht="19.5" customHeight="1">
-      <c r="A15" s="1" t="s">
+    </row>
+    <row r="15" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="6">
         <v>5000</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="5"/>
+    </row>
+    <row r="16" spans="1:18" ht="21" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="6">
+        <v>5000</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="9">
+        <f>B16+B8+B6+B9</f>
+        <v>11500</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="9">
+        <f>R2+R3</f>
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="9">
+        <f>D19-D20</f>
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="10">
+        <f>D19/D20</f>
+        <v>1.6428571428571428</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="10">
+        <f>R7/(R7+R6)</f>
+        <v>0.77272727272727271</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -920,7 +795,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -928,7 +803,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>